<commit_message>
[RTS DORA Incident Reporting] Small Fix (French+English)
Fixed the word "Recitals" in French and English
</commit_message>
<xml_diff>
--- a/tools/excel/dora/RTS/RTS-DORA-incident-reporting_official.xlsx
+++ b/tools/excel/dora/RTS/RTS-DORA-incident-reporting_official.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JulianDoloir\Desktop\Repos\intuitem\ciso-assistant-community\tools\excel\dora\RTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{730CD933-1443-4FC9-8BC7-24FA44CDD87E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA48EE3C-6EBC-4B77-A980-9E52DD2944F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-6620" yWindow="-19130" windowWidth="27180" windowHeight="17250" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-10410" yWindow="-21710" windowWidth="38620" windowHeight="21820" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_meta" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="285">
   <si>
     <t>type</t>
   </si>
@@ -86,9 +86,6 @@
   </si>
   <si>
     <t>assessable</t>
-  </si>
-  <si>
-    <t>Recital</t>
   </si>
   <si>
     <t>Recital 2</t>
@@ -270,9 +267,6 @@
     <t>1</t>
   </si>
   <si>
-    <t>recital</t>
-  </si>
-  <si>
     <t>2</t>
   </si>
   <si>
@@ -891,6 +885,15 @@
   <si>
     <t>Le présent règlement entre en vigueur le vingtième jour suivant celui de sa publication au Journal officiel de l’Union européenne.
 Le présent règlement est obligatoire dans tous ses éléments et directement applicable dans tout État membre.</t>
+  </si>
+  <si>
+    <t>Préambule</t>
+  </si>
+  <si>
+    <t>Recitals</t>
+  </si>
+  <si>
+    <t>recitals</t>
   </si>
 </sst>
 </file>
@@ -1010,7 +1013,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1059,6 +1062,9 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1631,7 +1637,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1655,7 +1661,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1663,7 +1669,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
@@ -1671,7 +1677,7 @@
         <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -1679,7 +1685,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -1687,7 +1693,7 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -1700,26 +1706,26 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" t="s">
         <v>70</v>
-      </c>
-      <c r="B13" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1754,7 +1760,7 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1762,7 +1768,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1770,7 +1776,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1786,23 +1792,23 @@
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -1814,7 +1820,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1835,7 +1841,7 @@
         <v>16</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>6</v>
@@ -1844,1572 +1850,1572 @@
         <v>7</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F1" s="9" t="s">
         <v>9</v>
       </c>
       <c r="G1" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="20" t="s">
         <v>61</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3"/>
       <c r="B2" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>77</v>
+        <v>283</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>284</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="16" t="s">
-        <v>17</v>
+        <v>282</v>
       </c>
       <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:8" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E3" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>81</v>
-      </c>
       <c r="G3" s="16" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="156" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="78" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
       <c r="B5" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E5" s="16" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E6" s="16" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="78" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="B7" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E7" s="16" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E8" s="16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A9" s="5"/>
       <c r="B9" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>24</v>
-      </c>
       <c r="G9" s="16" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="78" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
       <c r="B10" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E10" s="16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="78" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
       <c r="B11" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="F11" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="E11" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>97</v>
-      </c>
       <c r="G11" s="16" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="15"/>
       <c r="E13" s="16"/>
       <c r="F13" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G13" s="16"/>
       <c r="H13" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="16"/>
       <c r="F14" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G14" s="16"/>
       <c r="H14" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="16"/>
       <c r="F15" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G15" s="16"/>
       <c r="H15" s="5" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D16" s="15"/>
       <c r="E16" s="16"/>
       <c r="F16" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G16" s="16"/>
       <c r="H16" s="5" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="16"/>
       <c r="F17" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G17" s="16"/>
       <c r="H17" s="5" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D18" s="15"/>
       <c r="E18" s="16"/>
       <c r="F18" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G18" s="16"/>
       <c r="H18" s="5" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="16"/>
       <c r="F19" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G19" s="16"/>
       <c r="H19" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="16"/>
       <c r="F20" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G20" s="16"/>
       <c r="H20" s="5" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G21" s="18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="15"/>
       <c r="E22" s="16"/>
       <c r="F22" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G22" s="16"/>
       <c r="H22" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D23" s="15"/>
       <c r="E23" s="16"/>
       <c r="F23" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G23" s="16"/>
       <c r="H23" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D24" s="15"/>
       <c r="E24" s="16"/>
       <c r="F24" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G24" s="16"/>
       <c r="H24" s="5" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D25" s="15"/>
       <c r="E25" s="16"/>
       <c r="F25" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G25" s="16"/>
       <c r="H25" s="5" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D26" s="15"/>
       <c r="E26" s="16"/>
       <c r="F26" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G26" s="16"/>
       <c r="H26" s="5" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D27" s="15"/>
       <c r="E27" s="16"/>
       <c r="F27" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G27" s="16"/>
       <c r="H27" s="5" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D28" s="15"/>
       <c r="E28" s="16"/>
       <c r="F28" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G28" s="16"/>
       <c r="H28" s="5" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D29" s="15"/>
       <c r="E29" s="16"/>
       <c r="F29" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G29" s="16"/>
       <c r="H29" s="5" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D30" s="15"/>
       <c r="E30" s="16"/>
       <c r="F30" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G30" s="16"/>
       <c r="H30" s="5" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D31" s="15"/>
       <c r="E31" s="16"/>
       <c r="F31" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G31" s="16"/>
       <c r="H31" s="5" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D32" s="15"/>
       <c r="E32" s="16"/>
       <c r="F32" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G32" s="16"/>
       <c r="H32" s="5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="7"/>
       <c r="B33" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C33" s="6"/>
       <c r="D33" s="17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E33" s="18" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G33" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C34" s="8"/>
       <c r="D34" s="15"/>
       <c r="E34" s="16"/>
       <c r="F34" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G34" s="16"/>
       <c r="H34" s="5" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D35" s="15"/>
       <c r="E35" s="16"/>
       <c r="F35" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G35" s="16"/>
       <c r="H35" s="5" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D36" s="15"/>
       <c r="E36" s="16"/>
       <c r="F36" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G36" s="16"/>
       <c r="H36" s="5" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D37" s="15"/>
       <c r="E37" s="16"/>
       <c r="F37" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G37" s="16"/>
       <c r="H37" s="5" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D38" s="15"/>
       <c r="E38" s="16"/>
       <c r="F38" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G38" s="16"/>
       <c r="H38" s="5" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D39" s="15"/>
       <c r="E39" s="16"/>
       <c r="F39" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G39" s="16"/>
       <c r="H39" s="5" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D40" s="15"/>
       <c r="E40" s="16"/>
       <c r="F40" s="5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G40" s="16"/>
       <c r="H40" s="5" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D41" s="15"/>
       <c r="E41" s="16"/>
       <c r="F41" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G41" s="16"/>
       <c r="H41" s="5" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D42" s="15"/>
       <c r="E42" s="16"/>
       <c r="F42" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G42" s="16"/>
       <c r="H42" s="5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D43" s="15"/>
       <c r="E43" s="16"/>
       <c r="F43" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G43" s="16"/>
       <c r="H43" s="5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D44" s="15"/>
       <c r="E44" s="16"/>
       <c r="F44" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G44" s="16"/>
       <c r="H44" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D45" s="15"/>
       <c r="E45" s="16"/>
       <c r="F45" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G45" s="16"/>
       <c r="H45" s="5" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D46" s="15"/>
       <c r="E46" s="16"/>
       <c r="F46" s="5" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G46" s="16"/>
       <c r="H46" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="7"/>
       <c r="B47" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C47" s="6"/>
       <c r="D47" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E47" s="18" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G47" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A48" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C48" s="8"/>
       <c r="D48" s="15"/>
       <c r="E48" s="16"/>
       <c r="F48" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G48" s="16"/>
       <c r="H48" s="5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D49" s="15"/>
       <c r="E49" s="16"/>
       <c r="F49" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G49" s="16"/>
       <c r="H49" s="5" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D50" s="15"/>
       <c r="E50" s="16"/>
       <c r="F50" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G50" s="16"/>
       <c r="H50" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D51" s="15"/>
       <c r="E51" s="16"/>
       <c r="F51" s="5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G51" s="16"/>
       <c r="H51" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D52" s="15"/>
       <c r="E52" s="16"/>
       <c r="F52" s="5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G52" s="16"/>
       <c r="H52" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A53" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D53" s="15"/>
       <c r="E53" s="16"/>
       <c r="F53" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G53" s="16"/>
       <c r="H53" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D54" s="15"/>
       <c r="E54" s="16"/>
       <c r="F54" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G54" s="16"/>
       <c r="H54" s="5" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" s="7"/>
       <c r="B55" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C55" s="6"/>
       <c r="D55" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E55" s="18" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G55" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A56" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D56" s="15"/>
       <c r="E56" s="16"/>
       <c r="F56" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G56" s="16"/>
       <c r="H56" s="5" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A57" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D57" s="15"/>
       <c r="E57" s="16"/>
       <c r="F57" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G57" s="16"/>
       <c r="H57" s="5" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="78" x14ac:dyDescent="0.3">
       <c r="A58" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D58" s="15"/>
       <c r="E58" s="16"/>
       <c r="F58" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G58" s="16"/>
       <c r="H58" s="5" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A59" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D59" s="15"/>
       <c r="E59" s="16"/>
       <c r="F59" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G59" s="16"/>
       <c r="H59" s="5" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A60" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B60" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D60" s="15"/>
       <c r="E60" s="16"/>
       <c r="F60" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G60" s="16"/>
       <c r="H60" s="5" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A61" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B61" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D61" s="15"/>
       <c r="E61" s="16"/>
       <c r="F61" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G61" s="16"/>
       <c r="H61" s="5" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A62" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B62" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D62" s="15"/>
       <c r="E62" s="16"/>
       <c r="F62" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G62" s="16"/>
       <c r="H62" s="5" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A63" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B63" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D63" s="15"/>
       <c r="E63" s="16"/>
       <c r="F63" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G63" s="16"/>
       <c r="H63" s="5" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A64" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B64" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D64" s="15"/>
       <c r="E64" s="16"/>
       <c r="F64" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G64" s="16"/>
       <c r="H64" s="5" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A65" s="7"/>
       <c r="B65" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C65" s="6"/>
       <c r="D65" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E65" s="18" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G65" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H65" s="7" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C66" s="8"/>
       <c r="D66" s="15"/>
       <c r="E66" s="16"/>
       <c r="F66" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G66" s="16"/>
       <c r="H66" s="5" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D67" s="15"/>
       <c r="E67" s="16"/>
       <c r="F67" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G67" s="16"/>
       <c r="H67" s="5" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A68" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D68" s="15"/>
       <c r="E68" s="16"/>
       <c r="F68" s="5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G68" s="16"/>
       <c r="H68" s="5" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A69" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B69" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D69" s="15"/>
       <c r="E69" s="16"/>
       <c r="F69" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G69" s="16"/>
       <c r="H69" s="5" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A70" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D70" s="15"/>
       <c r="E70" s="16"/>
       <c r="F70" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G70" s="16"/>
       <c r="H70" s="5" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A71" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B71" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D71" s="15"/>
       <c r="E71" s="16"/>
       <c r="F71" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G71" s="16"/>
       <c r="H71" s="5" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A72" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D72" s="15"/>
       <c r="E72" s="16"/>
       <c r="F72" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G72" s="16"/>
       <c r="H72" s="5" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A73" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B73" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D73" s="15"/>
       <c r="E73" s="16"/>
       <c r="F73" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G73" s="16"/>
       <c r="H73" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A74" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B74" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D74" s="15"/>
       <c r="E74" s="16"/>
       <c r="F74" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G74" s="16"/>
       <c r="H74" s="5" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B75" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D75" s="15"/>
       <c r="E75" s="16"/>
       <c r="F75" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G75" s="16"/>
       <c r="H75" s="5" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A76" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B76" s="12" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D76" s="15"/>
       <c r="E76" s="16"/>
       <c r="F76" s="5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G76" s="16"/>
       <c r="H76" s="5" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="77" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A77" s="7"/>
       <c r="B77" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C77" s="6"/>
       <c r="D77" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E77" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="F77" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="E77" s="18" t="s">
-        <v>197</v>
-      </c>
-      <c r="F77" s="7" t="s">
-        <v>60</v>
-      </c>
       <c r="G77" s="18" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H77" s="7" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A78" s="5"/>
       <c r="B78" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C78" s="8"/>
       <c r="D78" s="15"/>
       <c r="E78" s="16"/>
       <c r="F78" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G78" s="16"/>
       <c r="H78" s="5" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
fix(lib): RTS DORA Incident Reporting Framework Text Layout Fix (#2562)
Fix Text Layout

Fixed a minor text layout issue in the description of Article 1 and its first point
</commit_message>
<xml_diff>
--- a/tools/excel/dora/RTS/RTS-DORA-incident-reporting_official.xlsx
+++ b/tools/excel/dora/RTS/RTS-DORA-incident-reporting_official.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JulianDoloir\Desktop\Repos\intuitem\ciso-assistant-community\tools\excel\dora\RTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA48EE3C-6EBC-4B77-A980-9E52DD2944F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29DEA4FD-44F2-4EF4-A854-A6B85CAF4409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10410" yWindow="-21710" windowWidth="38620" windowHeight="21820" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_meta" sheetId="1" r:id="rId1"/>
@@ -330,12 +330,6 @@
     <t>article-1</t>
   </si>
   <si>
-    <t>General information to be provided in initial notifications and intermediate and final reports on major ICT-</t>
-  </si>
-  <si>
-    <t>related incidents Financial entities shall include in the initial notification, the intermediate report, and the final report, as referred to in Article 19(4) of Regulation (EU) 2022/2554, the following general information:</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
@@ -688,12 +682,6 @@
     <t>Le Contrôleur européen de la protection des données a été consulté conformément à l’article 42, paragraphe 1, du règlement (UE) 2018/1725 du Parlement européen et du Conseil (6) et a rendu un avis positif le 22 juillet 2024. Tout traitement de données à caractère personnel relevant du champ d’application du présent règlement devrait être effectué conformément aux principes applicables en matière de protection des données et aux dispositions du règlement (UE) 2018/1725.</t>
   </si>
   <si>
-    <t>Informations générales à fournir dans les notifications initiales et les rapports intermédiaire et final sur les</t>
-  </si>
-  <si>
-    <t>incidents majeurs liés aux TIC Les entités financières incluent dans la notification initiale, le rapport intermédiaire et le rapport final, visés à l’article 19, paragraphe 4, du règlement (UE) 2022/2554, les informations générales suivantes:</t>
-  </si>
-  <si>
     <t>le type de soumission (notification initiale, rapport intermédiaire ou rapport final);</t>
   </si>
   <si>
@@ -894,6 +882,18 @@
   </si>
   <si>
     <t>recitals</t>
+  </si>
+  <si>
+    <t>Financial entities shall include in the initial notification, the intermediate report, and the final report, as referred to in Article 19(4) of Regulation (EU) 2022/2554, the following general information:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">General information to be provided in initial notifications and intermediate and final reports on major ICT-related incidents </t>
+  </si>
+  <si>
+    <t>Les entités financières incluent dans la notification initiale, le rapport intermédiaire et le rapport final, visés à l’article 19, paragraphe 4, du règlement (UE) 2022/2554, les informations générales suivantes:</t>
+  </si>
+  <si>
+    <t>Informations générales à fournir dans les notifications initiales et les rapports intermédiaire et final sur les incidents majeurs liés aux TIC</t>
   </si>
 </sst>
 </file>
@@ -1615,7 +1615,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1820,8 +1820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1869,14 +1869,14 @@
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="15" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="F2" s="3"/>
       <c r="G2" s="16" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="H2" s="3"/>
     </row>
@@ -1896,10 +1896,10 @@
         <v>79</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="156" x14ac:dyDescent="0.3">
@@ -1918,10 +1918,10 @@
         <v>81</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="78" x14ac:dyDescent="0.3">
@@ -1940,10 +1940,10 @@
         <v>83</v>
       </c>
       <c r="G5" s="16" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
@@ -1962,10 +1962,10 @@
         <v>85</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="78" x14ac:dyDescent="0.3">
@@ -1984,10 +1984,10 @@
         <v>87</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
@@ -2006,10 +2006,10 @@
         <v>89</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
@@ -2028,10 +2028,10 @@
         <v>23</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="78" x14ac:dyDescent="0.3">
@@ -2050,10 +2050,10 @@
         <v>92</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="78" x14ac:dyDescent="0.3">
@@ -2072,10 +2072,10 @@
         <v>95</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
@@ -2091,16 +2091,16 @@
         <v>96</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>97</v>
+        <v>282</v>
       </c>
       <c r="G12" s="18" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>26</v>
       </c>
@@ -2111,11 +2111,11 @@
       <c r="D13" s="15"/>
       <c r="E13" s="16"/>
       <c r="F13" s="5" t="s">
-        <v>98</v>
+        <v>281</v>
       </c>
       <c r="G13" s="16"/>
       <c r="H13" s="5" t="s">
-        <v>217</v>
+        <v>283</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -2123,19 +2123,19 @@
         <v>26</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="16"/>
       <c r="F14" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G14" s="16"/>
       <c r="H14" s="5" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
@@ -2143,19 +2143,19 @@
         <v>26</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="16"/>
       <c r="F15" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G15" s="16"/>
       <c r="H15" s="5" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
@@ -2163,19 +2163,19 @@
         <v>26</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D16" s="15"/>
       <c r="E16" s="16"/>
       <c r="F16" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G16" s="16"/>
       <c r="H16" s="5" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
@@ -2183,19 +2183,19 @@
         <v>26</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="16"/>
       <c r="F17" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G17" s="16"/>
       <c r="H17" s="5" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
@@ -2203,19 +2203,19 @@
         <v>26</v>
       </c>
       <c r="B18" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D18" s="15"/>
       <c r="E18" s="16"/>
       <c r="F18" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G18" s="16"/>
       <c r="H18" s="5" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
@@ -2223,19 +2223,19 @@
         <v>26</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="16"/>
       <c r="F19" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G19" s="16"/>
       <c r="H19" s="5" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -2243,19 +2243,19 @@
         <v>26</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="16"/>
       <c r="F20" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G20" s="16"/>
       <c r="H20" s="5" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -2268,16 +2268,16 @@
         <v>27</v>
       </c>
       <c r="E21" s="18" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G21" s="18" t="s">
         <v>27</v>
       </c>
       <c r="H21" s="7" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
@@ -2291,11 +2291,11 @@
       <c r="D22" s="15"/>
       <c r="E22" s="16"/>
       <c r="F22" s="5" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G22" s="16"/>
       <c r="H22" s="5" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -2303,7 +2303,7 @@
         <v>26</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>28</v>
@@ -2311,11 +2311,11 @@
       <c r="D23" s="15"/>
       <c r="E23" s="16"/>
       <c r="F23" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G23" s="16"/>
       <c r="H23" s="5" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
@@ -2323,7 +2323,7 @@
         <v>26</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>29</v>
@@ -2331,11 +2331,11 @@
       <c r="D24" s="15"/>
       <c r="E24" s="16"/>
       <c r="F24" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G24" s="16"/>
       <c r="H24" s="5" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -2343,7 +2343,7 @@
         <v>26</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>30</v>
@@ -2351,11 +2351,11 @@
       <c r="D25" s="15"/>
       <c r="E25" s="16"/>
       <c r="F25" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G25" s="16"/>
       <c r="H25" s="5" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
@@ -2363,7 +2363,7 @@
         <v>26</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>31</v>
@@ -2371,11 +2371,11 @@
       <c r="D26" s="15"/>
       <c r="E26" s="16"/>
       <c r="F26" s="5" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G26" s="16"/>
       <c r="H26" s="5" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -2383,7 +2383,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>32</v>
@@ -2391,11 +2391,11 @@
       <c r="D27" s="15"/>
       <c r="E27" s="16"/>
       <c r="F27" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G27" s="16"/>
       <c r="H27" s="5" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -2403,7 +2403,7 @@
         <v>26</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>33</v>
@@ -2411,11 +2411,11 @@
       <c r="D28" s="15"/>
       <c r="E28" s="16"/>
       <c r="F28" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G28" s="16"/>
       <c r="H28" s="5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -2423,7 +2423,7 @@
         <v>26</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>34</v>
@@ -2431,11 +2431,11 @@
       <c r="D29" s="15"/>
       <c r="E29" s="16"/>
       <c r="F29" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G29" s="16"/>
       <c r="H29" s="5" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -2443,19 +2443,19 @@
         <v>26</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D30" s="15"/>
       <c r="E30" s="16"/>
       <c r="F30" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G30" s="16"/>
       <c r="H30" s="5" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
@@ -2463,19 +2463,19 @@
         <v>26</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D31" s="15"/>
       <c r="E31" s="16"/>
       <c r="F31" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G31" s="16"/>
       <c r="H31" s="5" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -2483,19 +2483,19 @@
         <v>26</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D32" s="15"/>
       <c r="E32" s="16"/>
       <c r="F32" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G32" s="16"/>
       <c r="H32" s="5" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -2508,16 +2508,16 @@
         <v>35</v>
       </c>
       <c r="E33" s="18" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G33" s="18" t="s">
         <v>35</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
@@ -2531,11 +2531,11 @@
       <c r="D34" s="15"/>
       <c r="E34" s="16"/>
       <c r="F34" s="5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G34" s="16"/>
       <c r="H34" s="5" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -2543,7 +2543,7 @@
         <v>26</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>36</v>
@@ -2551,11 +2551,11 @@
       <c r="D35" s="15"/>
       <c r="E35" s="16"/>
       <c r="F35" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="G35" s="16"/>
       <c r="H35" s="5" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -2563,7 +2563,7 @@
         <v>26</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>37</v>
@@ -2571,11 +2571,11 @@
       <c r="D36" s="15"/>
       <c r="E36" s="16"/>
       <c r="F36" s="5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G36" s="16"/>
       <c r="H36" s="5" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -2583,7 +2583,7 @@
         <v>26</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>38</v>
@@ -2591,11 +2591,11 @@
       <c r="D37" s="15"/>
       <c r="E37" s="16"/>
       <c r="F37" s="5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G37" s="16"/>
       <c r="H37" s="5" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
@@ -2603,7 +2603,7 @@
         <v>26</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>39</v>
@@ -2611,11 +2611,11 @@
       <c r="D38" s="15"/>
       <c r="E38" s="16"/>
       <c r="F38" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G38" s="16"/>
       <c r="H38" s="5" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -2623,7 +2623,7 @@
         <v>26</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>40</v>
@@ -2631,11 +2631,11 @@
       <c r="D39" s="15"/>
       <c r="E39" s="16"/>
       <c r="F39" s="5" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G39" s="16"/>
       <c r="H39" s="5" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -2643,7 +2643,7 @@
         <v>26</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>41</v>
@@ -2651,11 +2651,11 @@
       <c r="D40" s="15"/>
       <c r="E40" s="16"/>
       <c r="F40" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G40" s="16"/>
       <c r="H40" s="5" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -2663,7 +2663,7 @@
         <v>26</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>42</v>
@@ -2675,7 +2675,7 @@
       </c>
       <c r="G41" s="16"/>
       <c r="H41" s="5" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -2683,7 +2683,7 @@
         <v>26</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>43</v>
@@ -2695,7 +2695,7 @@
       </c>
       <c r="G42" s="16"/>
       <c r="H42" s="5" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -2703,7 +2703,7 @@
         <v>26</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>44</v>
@@ -2715,7 +2715,7 @@
       </c>
       <c r="G43" s="16"/>
       <c r="H43" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -2723,7 +2723,7 @@
         <v>26</v>
       </c>
       <c r="B44" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>45</v>
@@ -2731,11 +2731,11 @@
       <c r="D44" s="15"/>
       <c r="E44" s="16"/>
       <c r="F44" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="G44" s="16"/>
       <c r="H44" s="5" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
@@ -2743,19 +2743,19 @@
         <v>26</v>
       </c>
       <c r="B45" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D45" s="15"/>
       <c r="E45" s="16"/>
       <c r="F45" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="G45" s="16"/>
       <c r="H45" s="5" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -2763,19 +2763,19 @@
         <v>26</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D46" s="15"/>
       <c r="E46" s="16"/>
       <c r="F46" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G46" s="16"/>
       <c r="H46" s="5" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -2788,16 +2788,16 @@
         <v>46</v>
       </c>
       <c r="E47" s="18" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G47" s="18" t="s">
         <v>46</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
@@ -2811,11 +2811,11 @@
       <c r="D48" s="15"/>
       <c r="E48" s="16"/>
       <c r="F48" s="5" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G48" s="16"/>
       <c r="H48" s="5" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -2823,7 +2823,7 @@
         <v>26</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>47</v>
@@ -2831,11 +2831,11 @@
       <c r="D49" s="15"/>
       <c r="E49" s="16"/>
       <c r="F49" s="5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G49" s="16"/>
       <c r="H49" s="5" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
@@ -2843,7 +2843,7 @@
         <v>26</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>48</v>
@@ -2851,11 +2851,11 @@
       <c r="D50" s="15"/>
       <c r="E50" s="16"/>
       <c r="F50" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G50" s="16"/>
       <c r="H50" s="5" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -2863,7 +2863,7 @@
         <v>26</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>49</v>
@@ -2871,11 +2871,11 @@
       <c r="D51" s="15"/>
       <c r="E51" s="16"/>
       <c r="F51" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G51" s="16"/>
       <c r="H51" s="5" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -2883,7 +2883,7 @@
         <v>26</v>
       </c>
       <c r="B52" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>50</v>
@@ -2891,11 +2891,11 @@
       <c r="D52" s="15"/>
       <c r="E52" s="16"/>
       <c r="F52" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G52" s="16"/>
       <c r="H52" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
@@ -2903,7 +2903,7 @@
         <v>26</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>51</v>
@@ -2911,11 +2911,11 @@
       <c r="D53" s="15"/>
       <c r="E53" s="16"/>
       <c r="F53" s="5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G53" s="16"/>
       <c r="H53" s="5" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -2923,7 +2923,7 @@
         <v>26</v>
       </c>
       <c r="B54" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>52</v>
@@ -2931,11 +2931,11 @@
       <c r="D54" s="15"/>
       <c r="E54" s="16"/>
       <c r="F54" s="5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G54" s="16"/>
       <c r="H54" s="5" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -2948,16 +2948,16 @@
         <v>56</v>
       </c>
       <c r="E55" s="18" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G55" s="18" t="s">
         <v>56</v>
       </c>
       <c r="H55" s="7" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
@@ -2968,16 +2968,16 @@
         <v>76</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D56" s="15"/>
       <c r="E56" s="16"/>
       <c r="F56" s="5" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G56" s="16"/>
       <c r="H56" s="5" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="46.8" x14ac:dyDescent="0.3">
@@ -2985,19 +2985,19 @@
         <v>26</v>
       </c>
       <c r="B57" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D57" s="15"/>
       <c r="E57" s="16"/>
       <c r="F57" s="5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G57" s="16"/>
       <c r="H57" s="5" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="78" x14ac:dyDescent="0.3">
@@ -3005,19 +3005,19 @@
         <v>26</v>
       </c>
       <c r="B58" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D58" s="15"/>
       <c r="E58" s="16"/>
       <c r="F58" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G58" s="16"/>
       <c r="H58" s="5" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
@@ -3025,19 +3025,19 @@
         <v>26</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D59" s="15"/>
       <c r="E59" s="16"/>
       <c r="F59" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="G59" s="16"/>
       <c r="H59" s="5" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
@@ -3048,16 +3048,16 @@
         <v>76</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D60" s="15"/>
       <c r="E60" s="16"/>
       <c r="F60" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G60" s="16"/>
       <c r="H60" s="5" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
@@ -3068,16 +3068,16 @@
         <v>76</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D61" s="15"/>
       <c r="E61" s="16"/>
       <c r="F61" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G61" s="16"/>
       <c r="H61" s="5" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
@@ -3088,16 +3088,16 @@
         <v>76</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D62" s="15"/>
       <c r="E62" s="16"/>
       <c r="F62" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G62" s="16"/>
       <c r="H62" s="5" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
@@ -3108,16 +3108,16 @@
         <v>76</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D63" s="15"/>
       <c r="E63" s="16"/>
       <c r="F63" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G63" s="16"/>
       <c r="H63" s="5" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="109.2" x14ac:dyDescent="0.3">
@@ -3128,16 +3128,16 @@
         <v>76</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D64" s="15"/>
       <c r="E64" s="16"/>
       <c r="F64" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G64" s="16"/>
       <c r="H64" s="5" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -3150,16 +3150,16 @@
         <v>57</v>
       </c>
       <c r="E65" s="18" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G65" s="18" t="s">
         <v>57</v>
       </c>
       <c r="H65" s="7" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
@@ -3173,11 +3173,11 @@
       <c r="D66" s="15"/>
       <c r="E66" s="16"/>
       <c r="F66" s="5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G66" s="16"/>
       <c r="H66" s="5" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -3185,19 +3185,19 @@
         <v>26</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D67" s="15"/>
       <c r="E67" s="16"/>
       <c r="F67" s="5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G67" s="16"/>
       <c r="H67" s="5" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
@@ -3205,19 +3205,19 @@
         <v>26</v>
       </c>
       <c r="B68" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D68" s="15"/>
       <c r="E68" s="16"/>
       <c r="F68" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G68" s="16"/>
       <c r="H68" s="5" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -3225,19 +3225,19 @@
         <v>26</v>
       </c>
       <c r="B69" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D69" s="15"/>
       <c r="E69" s="16"/>
       <c r="F69" s="5" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G69" s="16"/>
       <c r="H69" s="5" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
@@ -3245,19 +3245,19 @@
         <v>26</v>
       </c>
       <c r="B70" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D70" s="15"/>
       <c r="E70" s="16"/>
       <c r="F70" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G70" s="16"/>
       <c r="H70" s="5" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
@@ -3265,19 +3265,19 @@
         <v>26</v>
       </c>
       <c r="B71" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D71" s="15"/>
       <c r="E71" s="16"/>
       <c r="F71" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G71" s="16"/>
       <c r="H71" s="5" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
@@ -3285,19 +3285,19 @@
         <v>26</v>
       </c>
       <c r="B72" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D72" s="15"/>
       <c r="E72" s="16"/>
       <c r="F72" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G72" s="16"/>
       <c r="H72" s="5" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
@@ -3305,19 +3305,19 @@
         <v>26</v>
       </c>
       <c r="B73" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D73" s="15"/>
       <c r="E73" s="16"/>
       <c r="F73" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G73" s="16"/>
       <c r="H73" s="5" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
@@ -3325,19 +3325,19 @@
         <v>26</v>
       </c>
       <c r="B74" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D74" s="15"/>
       <c r="E74" s="16"/>
       <c r="F74" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G74" s="16"/>
       <c r="H74" s="5" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -3345,19 +3345,19 @@
         <v>26</v>
       </c>
       <c r="B75" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D75" s="15"/>
       <c r="E75" s="16"/>
       <c r="F75" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G75" s="16"/>
       <c r="H75" s="5" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -3365,19 +3365,19 @@
         <v>26</v>
       </c>
       <c r="B76" s="12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D76" s="15"/>
       <c r="E76" s="16"/>
       <c r="F76" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G76" s="16"/>
       <c r="H76" s="5" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="77" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -3390,7 +3390,7 @@
         <v>58</v>
       </c>
       <c r="E77" s="18" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F77" s="7" t="s">
         <v>59</v>
@@ -3399,7 +3399,7 @@
         <v>58</v>
       </c>
       <c r="H77" s="7" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
@@ -3411,11 +3411,11 @@
       <c r="D78" s="15"/>
       <c r="E78" s="16"/>
       <c r="F78" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G78" s="16"/>
       <c r="H78" s="5" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>